<commit_message>
Fixing typos and other little things
</commit_message>
<xml_diff>
--- a/files/schedule_modules.xlsx
+++ b/files/schedule_modules.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{7C40CE6C-DF63-484C-A234-8A007B7633E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2402478F-0A11-9A46-B13F-0C7B57C2BA50}"/>
   <bookViews>
-    <workbookView xWindow="17520" yWindow="5740" windowWidth="28800" windowHeight="16360" activeTab="2" xr2:uid="{21EBE61F-A4F0-3D45-865A-9EB87E85AA6A}"/>
+    <workbookView xWindow="17520" yWindow="5740" windowWidth="28800" windowHeight="16360" xr2:uid="{21EBE61F-A4F0-3D45-865A-9EB87E85AA6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="2" r:id="rId1"/>
@@ -479,7 +479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F342C0D-B564-AC4C-B9F2-1430BA1BF96D}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -684,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7AC0B77-377C-2E43-B142-D9BC271E0496}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -890,7 +890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48504950-6619-024D-BFE6-3D795EC0E695}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>